<commit_message>
Update BCRPP Incident Cases Correction Rules.xlsx
fixed size_primary# bug- size_primary# = 50 was being changed to sizecat_primary# = 3
</commit_message>
<xml_diff>
--- a/BCRPP_QC_R_Excel_Program/BCRPP_QC_Version_1/Incident Cases Rules/BCRPP Incident Cases Correction Rules.xlsx
+++ b/BCRPP_QC_R_Excel_Program/BCRPP_QC_Version_1/Incident Cases Rules/BCRPP Incident Cases Correction Rules.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10311"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F10BF0-EDE9-0F4F-8DDD-7A96E1165B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9134559A-33D3-DD48-9D14-9EC2A8E23727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -88,9 +88,6 @@
     <t>sizecat_primary1 != 3</t>
   </si>
   <si>
-    <t>size_primary1 &gt;= 50 &amp; size_primary1 != 888 &amp; size_primary1 != 777</t>
-  </si>
-  <si>
     <t>sizecat_primary1 changed to 3 (size_primary1 is greater than 5 cm)</t>
   </si>
   <si>
@@ -121,9 +118,6 @@
     <t>sizecat_primary2 changed to 2 (size_primary2 is between 2 and 5  cm)</t>
   </si>
   <si>
-    <t>size_primary2 &gt;= 50 &amp; size_primary2 != 888 &amp; size_primary2 != 777</t>
-  </si>
-  <si>
     <t>sizecat_primary2 changed to 3 (size_primary2 is greater than 5 cm)</t>
   </si>
   <si>
@@ -140,6 +134,12 @@
   </si>
   <si>
     <t>dxdate_primary2 changed to 7777 from 777 to match data dictionary</t>
+  </si>
+  <si>
+    <t>size_primary1 &gt;50 &amp; size_primary1 != 888 &amp; size_primary1 != 777</t>
+  </si>
+  <si>
+    <t>size_primary2 &gt; 50 &amp; size_primary2 != 888 &amp; size_primary2 != 777</t>
   </si>
 </sst>
 </file>
@@ -507,7 +507,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -628,116 +628,116 @@
         <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="L4">
         <v>3</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
         <v>25</v>
-      </c>
-      <c r="B5" t="s">
-        <v>26</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
       </c>
       <c r="D5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" t="s">
         <v>29</v>
-      </c>
-      <c r="E5" t="s">
-        <v>30</v>
       </c>
       <c r="L5">
         <v>1</v>
       </c>
       <c r="M5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L6">
         <v>2</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="L7">
         <v>3</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B8">
         <v>777</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L8">
         <v>7777</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B9">
         <v>777</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L9">
         <v>7777</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>